<commit_message>
feat: :sparkles: Added the PopUp componente to error management
</commit_message>
<xml_diff>
--- a/node/Historico.xlsx
+++ b/node/Historico.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="47">
   <si>
     <t>Area</t>
   </si>
@@ -34,37 +34,124 @@
     <t>Equipo</t>
   </si>
   <si>
-    <t>Cyber</t>
+    <t>Nano</t>
+  </si>
+  <si>
+    <t>Prototipo</t>
+  </si>
+  <si>
+    <t>bgjonbipga´dnj´goa</t>
+  </si>
+  <si>
+    <t>Marlon Yahir Martínez</t>
+  </si>
+  <si>
+    <t>FAS</t>
+  </si>
+  <si>
+    <t>Prototipo finalizado</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>fsa</t>
+  </si>
+  <si>
+    <t>fas</t>
+  </si>
+  <si>
+    <t>fsaf</t>
+  </si>
+  <si>
+    <t>Proyecto para pbrar el commit de gerry</t>
+  </si>
+  <si>
+    <t>fsfa</t>
+  </si>
+  <si>
+    <t>fasfa</t>
+  </si>
+  <si>
+    <t>Bio</t>
+  </si>
+  <si>
+    <t>Otra nueva actualización</t>
+  </si>
+  <si>
+    <t>video123</t>
+  </si>
+  <si>
+    <t>poster123</t>
+  </si>
+  <si>
+    <t>Proyecto de prueba para autorizar</t>
+  </si>
+  <si>
+    <t>Prueba de que funciona</t>
+  </si>
+  <si>
+    <t>fasfsa</t>
+  </si>
+  <si>
+    <t>fsafas</t>
+  </si>
+  <si>
+    <t>Proyecto de prueba</t>
+  </si>
+  <si>
+    <t>video.pdf</t>
+  </si>
+  <si>
+    <t>poster.pdf</t>
+  </si>
+  <si>
+    <t>Nexus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esto funcionara </t>
+  </si>
+  <si>
+    <t>fsfafsa</t>
+  </si>
+  <si>
+    <t>fad</t>
+  </si>
+  <si>
+    <t>fasfaf</t>
+  </si>
+  <si>
+    <t>fsafa</t>
   </si>
   <si>
     <t>Concepto</t>
   </si>
   <si>
-    <t>Proyecto A</t>
-  </si>
-  <si>
-    <t>Marlon Martínez</t>
-  </si>
-  <si>
-    <t>https://youtu.be/fFHlfbKVi30?si=L24uiVr-kFUA0eEP</t>
-  </si>
-  <si>
-    <t>linkPoster</t>
-  </si>
-  <si>
-    <t>nuevofdsgsadgsdgasg</t>
-  </si>
-  <si>
-    <t>Nano</t>
-  </si>
-  <si>
-    <t>Proyecto B</t>
+    <t>Prueba para certificados no lo borren</t>
+  </si>
+  <si>
+    <t>Sarai Santiago Lozano</t>
+  </si>
+  <si>
+    <t>holaaaaaaaa2</t>
+  </si>
+  <si>
+    <t>holaaaaa</t>
+  </si>
+  <si>
+    <t>Robot automata para automatizar automatas</t>
   </si>
   <si>
     <t>Gerry Deustúa Hernández</t>
   </si>
   <si>
-    <t>Proyecto de prueba 2</t>
+    <t>DBDFBDFB</t>
+  </si>
+  <si>
+    <t>HDD</t>
+  </si>
+  <si>
+    <t>BOLDBGOSDBGOSANGSIGNSOPGSDG</t>
   </si>
 </sst>
 </file>
@@ -454,7 +541,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G12"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="7" width="30" customWidth="1"/>
@@ -500,33 +587,240 @@
         <v>11</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="F3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>17</v>
+      <c r="C10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
perf: :zap: improbed files management for areas and projects
</commit_message>
<xml_diff>
--- a/node/Historico.xlsx
+++ b/node/Historico.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>Area</t>
   </si>
@@ -37,61 +37,76 @@
     <t>Nano</t>
   </si>
   <si>
+    <t>Prototipo</t>
+  </si>
+  <si>
+    <t>Titulo para mi proyecto de prubas Gerry</t>
+  </si>
+  <si>
+    <t>Gerry Deustúa Hernández</t>
+  </si>
+  <si>
+    <t>BOLDBGOSDBGOSANGSIGNSOPGSDG</t>
+  </si>
+  <si>
+    <t>Concepto</t>
+  </si>
+  <si>
+    <t>Test89</t>
+  </si>
+  <si>
+    <t>Mikel Edel</t>
+  </si>
+  <si>
+    <t>rrrrrrrrrr</t>
+  </si>
+  <si>
+    <t>aaaaaaa</t>
+  </si>
+  <si>
     <t>Prototipo finalizado</t>
   </si>
   <si>
-    <t>Proyecto para pbrar el commit de gerry</t>
-  </si>
-  <si>
-    <t>Marlon Yahir Martínez</t>
+    <t>Proyecto de prueba</t>
+  </si>
+  <si>
+    <t>Marlon Martínez</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>Nexus</t>
   </si>
   <si>
     <t>fsfa</t>
   </si>
   <si>
-    <t>fasfa</t>
-  </si>
-  <si>
-    <t>Prototipo</t>
-  </si>
-  <si>
-    <t>Prueb 1</t>
-  </si>
-  <si>
-    <t>Cesar Guerra Martinez</t>
-  </si>
-  <si>
-    <t>xyxtydtytyy89y</t>
-  </si>
-  <si>
-    <t>iyiulllgyuttu</t>
+    <t>fasfsa</t>
+  </si>
+  <si>
+    <t>fsa</t>
+  </si>
+  <si>
+    <t>Robot automata para automatizar automatas</t>
+  </si>
+  <si>
+    <t>sdgasdgasdg</t>
+  </si>
+  <si>
+    <t>sadgsadg</t>
   </si>
   <si>
     <t>Cyber</t>
   </si>
   <si>
-    <t>Ale Hugo Zago</t>
-  </si>
-  <si>
-    <t>lmao.com/youtube</t>
-  </si>
-  <si>
-    <t>lmao.com</t>
-  </si>
-  <si>
-    <t>Concepto</t>
-  </si>
-  <si>
-    <t>Test 123</t>
-  </si>
-  <si>
-    <t>Mikel Edel</t>
-  </si>
-  <si>
-    <t>asdsadasdsa</t>
-  </si>
-  <si>
-    <t>asdadasa</t>
+    <t>dsfomo´ghdsrg</t>
+  </si>
+  <si>
+    <t>dgfgj sdlgondskgdsfg</t>
+  </si>
+  <si>
+    <t>df´pdsfkg´pdgksdg</t>
   </si>
 </sst>
 </file>
@@ -481,7 +496,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="7" width="30" customWidth="1"/>
@@ -527,7 +542,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>9</v>
@@ -538,32 +553,34 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="G3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
         <v>19</v>
       </c>
@@ -571,31 +588,79 @@
         <v>20</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="G5" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>23</v>
+      <c r="F6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: :sparkles: In-place rubric modification
</commit_message>
<xml_diff>
--- a/node/Historico.xlsx
+++ b/node/Historico.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
     <t>Area</t>
   </si>
@@ -22,6 +22,9 @@
     <t>Proyecto</t>
   </si>
   <si>
+    <t>Calificación</t>
+  </si>
+  <si>
     <t>Lider</t>
   </si>
   <si>
@@ -34,6 +37,24 @@
     <t>Equipo</t>
   </si>
   <si>
+    <t>Cyber</t>
+  </si>
+  <si>
+    <t>Concepto</t>
+  </si>
+  <si>
+    <t>dsfomo´ghdsrg</t>
+  </si>
+  <si>
+    <t>Marlon Martínez</t>
+  </si>
+  <si>
+    <t>dgfgj sdlgondskgdsfg</t>
+  </si>
+  <si>
+    <t>df´pdsfkg´pdgksdg</t>
+  </si>
+  <si>
     <t>Nano</t>
   </si>
   <si>
@@ -43,15 +64,15 @@
     <t>Titulo para mi proyecto de prubas Gerry</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>Gerry Deustúa Hernández</t>
   </si>
   <si>
     <t>BOLDBGOSDBGOSANGSIGNSOPGSDG</t>
   </si>
   <si>
-    <t>Concepto</t>
-  </si>
-  <si>
     <t>Test89</t>
   </si>
   <si>
@@ -64,21 +85,27 @@
     <t>aaaaaaa</t>
   </si>
   <si>
-    <t>Prototipo finalizado</t>
+    <t>Nexus</t>
+  </si>
+  <si>
+    <t>Robot automata para automatizar automatas</t>
+  </si>
+  <si>
+    <t>sdgasdgasdg</t>
+  </si>
+  <si>
+    <t>sadgsadg</t>
+  </si>
+  <si>
+    <t>Producto</t>
   </si>
   <si>
     <t>Proyecto de prueba</t>
   </si>
   <si>
-    <t>Marlon Martínez</t>
-  </si>
-  <si>
     <t>link</t>
   </si>
   <si>
-    <t>Nexus</t>
-  </si>
-  <si>
     <t>fsfa</t>
   </si>
   <si>
@@ -86,27 +113,6 @@
   </si>
   <si>
     <t>fsa</t>
-  </si>
-  <si>
-    <t>Robot automata para automatizar automatas</t>
-  </si>
-  <si>
-    <t>sdgasdgasdg</t>
-  </si>
-  <si>
-    <t>sadgsadg</t>
-  </si>
-  <si>
-    <t>Cyber</t>
-  </si>
-  <si>
-    <t>dsfomo´ghdsrg</t>
-  </si>
-  <si>
-    <t>dgfgj sdlgondskgdsfg</t>
-  </si>
-  <si>
-    <t>df´pdsfkg´pdgksdg</t>
   </si>
 </sst>
 </file>
@@ -496,13 +502,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="7" width="30" customWidth="1"/>
+    <col min="1" max="8" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -524,143 +530,164 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="D2" s="3">
+        <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>9</v>
+      <c r="F6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: :zap: historico data improved
</commit_message>
<xml_diff>
--- a/node/Historico.xlsx
+++ b/node/Historico.xlsx
@@ -13,6 +13,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
+    <t>Id</t>
+  </si>
+  <si>
     <t>Area</t>
   </si>
   <si>
@@ -37,42 +40,69 @@
     <t>Equipo</t>
   </si>
   <si>
-    <t>Cyber</t>
+    <t>BioPro1</t>
+  </si>
+  <si>
+    <t>Bio</t>
+  </si>
+  <si>
+    <t>Prototipo</t>
+  </si>
+  <si>
+    <t>Titulo para mi proyecto de prubas p</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Gerardo Deustúa Hernández</t>
+  </si>
+  <si>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>NexPro2</t>
+  </si>
+  <si>
+    <t>Nexus</t>
+  </si>
+  <si>
+    <t>Producto</t>
+  </si>
+  <si>
+    <t>sfsdfbdsfb</t>
+  </si>
+  <si>
+    <t>Robot automata para automatizar automatas</t>
+  </si>
+  <si>
+    <t>NexCon1</t>
   </si>
   <si>
     <t>Concepto</t>
   </si>
   <si>
-    <t>dsfomo´ghdsrg</t>
-  </si>
-  <si>
-    <t>Marlon Martínez</t>
-  </si>
-  <si>
-    <t>dgfgj sdlgondskgdsfg</t>
-  </si>
-  <si>
-    <t>df´pdsfkg´pdgksdg</t>
+    <t>sdgasdgasdg</t>
+  </si>
+  <si>
+    <t>sadgsadg</t>
+  </si>
+  <si>
+    <t>NanPro2</t>
   </si>
   <si>
     <t>Nano</t>
   </si>
   <si>
-    <t>Prototipo</t>
-  </si>
-  <si>
     <t>Titulo para mi proyecto de prubas Gerry</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>Gerry Deustúa Hernández</t>
-  </si>
-  <si>
     <t>BOLDBGOSDBGOSANGSIGNSOPGSDG</t>
   </si>
   <si>
+    <t>NanCon1</t>
+  </si>
+  <si>
     <t>Test89</t>
   </si>
   <si>
@@ -83,36 +113,6 @@
   </si>
   <si>
     <t>aaaaaaa</t>
-  </si>
-  <si>
-    <t>Nexus</t>
-  </si>
-  <si>
-    <t>Robot automata para automatizar automatas</t>
-  </si>
-  <si>
-    <t>sdgasdgasdg</t>
-  </si>
-  <si>
-    <t>sadgsadg</t>
-  </si>
-  <si>
-    <t>Producto</t>
-  </si>
-  <si>
-    <t>Proyecto de prueba</t>
-  </si>
-  <si>
-    <t>link</t>
-  </si>
-  <si>
-    <t>fsfa</t>
-  </si>
-  <si>
-    <t>fasfsa</t>
-  </si>
-  <si>
-    <t>fsa</t>
   </si>
 </sst>
 </file>
@@ -502,13 +502,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="8" width="30" customWidth="1"/>
+    <col min="1" max="9" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -533,161 +533,153 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>10</v>
+      <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>23</v>
       </c>
       <c r="H4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="C6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="3">
-        <v>3.2</v>
+        <v>22</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>